<commit_message>
Translate newdir/test.xlsx in de_DE
100% translated source file: 'newdir/test.xlsx'
on 'de_DE'.
</commit_message>
<xml_diff>
--- a/Τranslations/test1_de_DE.xlsx
+++ b/Τranslations/test1_de_DE.xlsx
@@ -356,7 +356,7 @@
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>testen</t>
+          <t>test 1 fr</t>
         </is>
       </c>
       <c r="I2" s="1" t="inlineStr">
@@ -386,9 +386,14 @@
           <t>example</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Beispiel</t>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>test 1 fr</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="inlineStr">
+        <is>
+          <t>test 1 fr</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -418,9 +423,14 @@
           <t>fish</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>angeln</t>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>test 1 fr</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="inlineStr">
+        <is>
+          <t>test 1 fr</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">

</xml_diff>

<commit_message>
Translate newdir/test.xlsx in de_DE [Manual Sync]
100% translated source file: 'newdir/test.xlsx'
on 'de_DE'.
</commit_message>
<xml_diff>
--- a/Τranslations/test1_de_DE.xlsx
+++ b/Τranslations/test1_de_DE.xlsx
@@ -364,7 +364,7 @@
           <t>test</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J2" s="0" t="inlineStr">
         <is>
           <t>2023-11-09</t>
         </is>
@@ -416,7 +416,7 @@
           <t>test</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="J3" s="0" t="inlineStr">
         <is>
           <t>2023-11-09</t>
         </is>
@@ -468,7 +468,7 @@
           <t>test</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="J4" s="0" t="inlineStr">
         <is>
           <t>2023-11-09</t>
         </is>

</xml_diff>